<commit_message>
This commit updates the Excel files in readme
</commit_message>
<xml_diff>
--- a/assets/readme/Milestoneonetesting.xlsx
+++ b/assets/readme/Milestoneonetesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattjones/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3F05145-12F7-1946-9C17-A2762BED2567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EBF31E-5D68-C84D-A50B-2DDE28FEAE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14180" xr2:uid="{45F18A2D-9174-0E41-8333-BA2DF8A9637B}"/>
   </bookViews>
@@ -275,18 +275,18 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,7 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5531694B-5253-B345-8135-12EF323D74FD}">
   <dimension ref="B3:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -643,535 +643,575 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
       <c r="F9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
       <c r="F11" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
       <c r="F12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="F14" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="F15" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="F17" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
       <c r="F18" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="5"/>
       <c r="F20" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="5"/>
       <c r="F21" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
       <c r="F23" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
       <c r="F24" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="F27" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
       <c r="F29" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
       <c r="F30" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
       <c r="F32" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
       <c r="F33" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
       <c r="F35" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
       <c r="F36" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
       <c r="F38" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
       <c r="F39" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E31:E33"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="D34:D36"/>
@@ -1180,46 +1220,6 @@
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="E37:E39"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>